<commit_message>
Formularios Parcial 1 AIC
</commit_message>
<xml_diff>
--- a/3º/Notas 3r.xlsx
+++ b/3º/Notas 3r.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismael/Documents/GitHub/Ingenieria-Informatica/3º/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0F854A-5F65-244F-B08C-748AA1E6CE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E265AB5-EC0A-D94E-AC75-6A6F3BA49E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="1740" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1098,8 +1098,8 @@
   </sheetPr>
   <dimension ref="A1:AF87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:AF8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1168,40 +1168,46 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6">
+        <v>7.91</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4.8</v>
+      </c>
       <c r="D2" s="2">
         <f>B2+C2</f>
-        <v>0</v>
+        <v>12.71</v>
       </c>
       <c r="E2" s="6">
         <f t="shared" ref="E2:F2" si="0">B2*0.3</f>
-        <v>0</v>
+        <v>2.3729999999999998</v>
       </c>
       <c r="F2" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.44</v>
       </c>
       <c r="G2" s="2">
         <f>F2+E2</f>
-        <v>0</v>
+        <v>3.8129999999999997</v>
       </c>
       <c r="H2" s="6">
         <f>B2*0.1</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="6"/>
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.6</v>
+      </c>
       <c r="J2" s="6">
         <f>C2*0.1</f>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="K2" s="2">
         <f>H2+I2+J2</f>
-        <v>0</v>
+        <v>1.871</v>
       </c>
       <c r="L2" s="2">
         <f>G2+K2</f>
-        <v>0</v>
+        <v>5.6839999999999993</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -1717,11 +1723,11 @@
         <v>4</v>
       </c>
       <c r="C14" s="28">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="D14" s="24">
         <f>(B14+C14)*0.7/2</f>
-        <v>2.8</v>
+        <v>2.52</v>
       </c>
       <c r="E14" s="28">
         <v>3.94</v>
@@ -1766,7 +1772,7 @@
       </c>
       <c r="R14" s="24">
         <f>D14+I14+Q14</f>
-        <v>4.9432142857142862</v>
+        <v>4.663214285714286</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>

</xml_diff>